<commit_message>
change base url and add ssh url
</commit_message>
<xml_diff>
--- a/public/sample/farmer.xlsx
+++ b/public/sample/farmer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itsam\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2712315-B2A1-4F6F-9611-87F0CD63EE2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1FA0FD-6E66-416B-8AAD-43D07D2C1BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="21624" windowHeight="11124" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>name</t>
   </si>
@@ -34,6 +34,21 @@
   </si>
   <si>
     <t>Rajjuu</t>
+  </si>
+  <si>
+    <t>village</t>
+  </si>
+  <si>
+    <t>block</t>
+  </si>
+  <si>
+    <t>asdad</t>
+  </si>
+  <si>
+    <t>asdsa</t>
+  </si>
+  <si>
+    <t>land_area</t>
   </si>
 </sst>
 </file>
@@ -351,32 +366,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>9868638507</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
paroduct module chnages from userid to jwt
</commit_message>
<xml_diff>
--- a/public/sample/farmer.xlsx
+++ b/public/sample/farmer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itsam\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\backe\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1FA0FD-6E66-416B-8AAD-43D07D2C1BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604B5421-DE96-49F4-B915-F95A818433A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>name</t>
   </si>
@@ -48,7 +48,10 @@
     <t>asdsa</t>
   </si>
   <si>
-    <t>land_area</t>
+    <t>district</t>
+  </si>
+  <si>
+    <t>Aligarh</t>
   </si>
 </sst>
 </file>
@@ -410,8 +413,8 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="E2">
-        <v>40</v>
+      <c r="E2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>